<commit_message>
IMPLEMENTASI POS: Update Perbaikan Typo ✨
</commit_message>
<xml_diff>
--- a/POS/public/template_user.xlsx
+++ b/POS/public/template_user.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_Ghetsa-Ramadhani\POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8AF63A-3A06-47E4-9918-C7083EF3C7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E054A5F-1072-45BF-BA98-DE2F4FFA05AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="15720" windowHeight="11850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-83" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -448,7 +451,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -469,8 +472,8 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">

</xml_diff>